<commit_message>
Change field name to program_registration_id
</commit_message>
<xml_diff>
--- a/backend/hct_mis_api/apps/core/tests/test_files/kobo-template-valid.xlsx
+++ b/backend/hct_mis_api/apps/core/tests/test_files/kobo-template-valid.xlsx
@@ -7423,10 +7423,10 @@
     <t xml:space="preserve">What is the Family’s average daily income in ${currency_h_c} </t>
   </si>
   <si>
-    <t>kobo_registration_id_h_c</t>
-  </si>
-  <si>
-    <t>Kobo registration id</t>
+    <t>program_registration_id_h_c</t>
+  </si>
+  <si>
+    <t>Program registration id</t>
   </si>
   <si>
     <t>form_title</t>
@@ -8524,13 +8524,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -8628,10 +8622,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -8877,13 +8871,7 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
+        <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -9185,10 +9173,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">

</xml_diff>